<commit_message>
All File are updated
</commit_message>
<xml_diff>
--- a/download/Purchase Order (purchase.order).xlsx
+++ b/download/Purchase Order (purchase.order).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Company</t>
   </si>
@@ -76,49 +76,46 @@
     <t>Shipment Mode</t>
   </si>
   <si>
-    <t>USD (1)</t>
-  </si>
-  <si>
-    <t>22908.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    raw (1)</t>
-  </si>
-  <si>
-    <t>Metal Trims</t>
-  </si>
-  <si>
-    <t>Tanmim Akter</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Suranjan Kumar</t>
-  </si>
-  <si>
-    <t>P17695</t>
+    <t>Zipper (1)</t>
+  </si>
+  <si>
+    <t>274000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    BDT (1)</t>
+  </si>
+  <si>
+    <t>Zipper</t>
+  </si>
+  <si>
+    <t>Shamsuddin Ahamed</t>
+  </si>
+  <si>
+    <t>BDT</t>
+  </si>
+  <si>
+    <t>MD. MONIR HOSSAIN</t>
+  </si>
+  <si>
+    <t>Md. Shahid Hossain</t>
+  </si>
+  <si>
+    <t>P18037</t>
   </si>
   <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>Forecasting for May</t>
-  </si>
-  <si>
-    <t>To Approve</t>
-  </si>
-  <si>
-    <t>Shanghai Wuxing Copper Co. Ltd.</t>
-  </si>
-  <si>
-    <t>[CFR] COST AND FREIGHT</t>
-  </si>
-  <si>
-    <t>[R_1_002_01_034] Brass Strip-0.30x305mm-soft</t>
-  </si>
-  <si>
-    <t>Sea</t>
+    <t>Dyeing CIP (Mr Anup)</t>
+  </si>
+  <si>
+    <t>RFQ Sent</t>
+  </si>
+  <si>
+    <t>Vision Tex CO</t>
+  </si>
+  <si>
+    <t>By Road</t>
   </si>
 </sst>
 </file>
@@ -609,7 +606,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="4">
-        <v>45754.50240740741</v>
+        <v>45806.60496527778</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>25</v>
@@ -620,41 +617,39 @@
       <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="4">
-        <v>45804.57181712963</v>
+        <v>45806.72810185186</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="3">
-        <v>22908</v>
+        <v>274000</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>